<commit_message>
add emdat panel data
</commit_message>
<xml_diff>
--- a/data/meta_dhs_mics_updated.xlsx
+++ b/data/meta_dhs_mics_updated.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annapalmer/Documents/GitHub/cyclone-child-marraige/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BA3B90-9FB9-FA43-B1A8-5AEF54EDF3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3DCE438-4425-A246-8DA3-96CC9FC38184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5680" yWindow="500" windowWidth="44300" windowHeight="25280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5680" yWindow="500" windowWidth="48620" windowHeight="25280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="384">
   <si>
     <t>iso</t>
   </si>
@@ -1173,6 +1173,18 @@
   </si>
   <si>
     <t>end_yr</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>st_yr</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>ed_yr</t>
   </si>
 </sst>
 </file>
@@ -1233,9 +1245,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1540,11 +1550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P122"/>
+  <dimension ref="A1:S122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M107" sqref="M107"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1558,13 +1568,16 @@
     <col min="8" max="8" width="8.83203125" style="2"/>
     <col min="9" max="9" width="10.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="56.1640625" style="2" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" style="2"/>
-    <col min="13" max="13" width="15.83203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="44.5" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="2"/>
+    <col min="11" max="11" width="9.83203125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.6640625" style="2" customWidth="1"/>
+    <col min="14" max="15" width="8.83203125" style="2"/>
+    <col min="16" max="16" width="15.83203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="44.5" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1595,26 +1608,35 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -1639,8 +1661,17 @@
       <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1980</v>
+      </c>
+      <c r="M2">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1671,8 +1702,17 @@
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1981</v>
+      </c>
+      <c r="M3">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -1703,8 +1743,17 @@
       <c r="J4" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>1980</v>
+      </c>
+      <c r="M4">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
@@ -1726,8 +1775,13 @@
       <c r="I5" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>382</v>
+      </c>
+      <c r="L5"/>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1755,8 +1809,17 @@
       <c r="J6" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>1980</v>
+      </c>
+      <c r="M6">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>26</v>
       </c>
@@ -1781,8 +1844,17 @@
       <c r="I7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <v>1980</v>
+      </c>
+      <c r="M7">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
@@ -1813,8 +1885,17 @@
       <c r="J8" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>1980</v>
+      </c>
+      <c r="M8">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>34</v>
       </c>
@@ -1845,8 +1926,17 @@
       <c r="J9" s="2" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1980</v>
+      </c>
+      <c r="M9">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>38</v>
       </c>
@@ -1877,8 +1967,17 @@
       <c r="J10" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <v>1980</v>
+      </c>
+      <c r="M10">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>42</v>
       </c>
@@ -1909,20 +2008,29 @@
       <c r="J11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="3">
-        <v>1</v>
-      </c>
-      <c r="L11" s="3" t="s">
+      <c r="K11">
+        <v>2</v>
+      </c>
+      <c r="L11">
+        <v>1980</v>
+      </c>
+      <c r="M11">
+        <v>2015</v>
+      </c>
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="O11" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P11" s="3">
+      <c r="R11" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S11" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>47</v>
       </c>
@@ -1944,8 +2052,13 @@
       <c r="I12" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K12" t="s">
+        <v>382</v>
+      </c>
+      <c r="L12"/>
+      <c r="M12"/>
+    </row>
+    <row r="13" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>48</v>
       </c>
@@ -1970,8 +2083,17 @@
       <c r="I13" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>1980</v>
+      </c>
+      <c r="M13">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -1996,23 +2118,32 @@
       <c r="I14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="3">
-        <v>1</v>
-      </c>
-      <c r="L14" s="3" t="s">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1980</v>
+      </c>
+      <c r="M14">
+        <v>2012</v>
+      </c>
+      <c r="N14" s="3">
+        <v>1</v>
+      </c>
+      <c r="O14" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="N14" s="3" t="s">
+      <c r="Q14" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="O14" s="3">
+      <c r="R14" s="3">
         <v>2003</v>
       </c>
-      <c r="P14" s="3">
+      <c r="S14" s="3">
         <v>2012</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -2043,8 +2174,17 @@
       <c r="J15" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>1980</v>
+      </c>
+      <c r="M15">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>59</v>
       </c>
@@ -2066,14 +2206,19 @@
       <c r="I16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K16" s="2">
-        <v>1</v>
-      </c>
-      <c r="M16" s="2" t="s">
+      <c r="K16" t="s">
+        <v>382</v>
+      </c>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16" s="2">
+        <v>1</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>60</v>
       </c>
@@ -2095,14 +2240,19 @@
       <c r="I17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K17" s="2">
-        <v>1</v>
-      </c>
-      <c r="M17" s="2" t="s">
+      <c r="K17" t="s">
+        <v>382</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17" s="2">
+        <v>1</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>61</v>
       </c>
@@ -2127,8 +2277,17 @@
       <c r="I18" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1980</v>
+      </c>
+      <c r="M18">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
@@ -2159,8 +2318,17 @@
       <c r="J19" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="20" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1980</v>
+      </c>
+      <c r="M19">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>69</v>
       </c>
@@ -2191,8 +2359,17 @@
       <c r="J20" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1980</v>
+      </c>
+      <c r="M20">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
@@ -2223,8 +2400,17 @@
       <c r="J21" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>1980</v>
+      </c>
+      <c r="M21">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>79</v>
       </c>
@@ -2255,8 +2441,17 @@
       <c r="J22" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1980</v>
+      </c>
+      <c r="M22">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>83</v>
       </c>
@@ -2281,8 +2476,17 @@
       <c r="I23" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1980</v>
+      </c>
+      <c r="M23">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>86</v>
       </c>
@@ -2313,8 +2517,17 @@
       <c r="J24" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>1980</v>
+      </c>
+      <c r="M24">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>89</v>
       </c>
@@ -2342,20 +2555,29 @@
       <c r="J25" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="K25" s="3">
-        <v>1</v>
-      </c>
-      <c r="L25" s="3" t="s">
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>1980</v>
+      </c>
+      <c r="M25">
+        <v>2008</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1</v>
+      </c>
+      <c r="O25" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O25" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P25" s="3">
+      <c r="R25" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S25" s="3">
         <v>2008</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>92</v>
       </c>
@@ -2380,8 +2602,17 @@
       <c r="I26" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>1980</v>
+      </c>
+      <c r="M26">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>95</v>
       </c>
@@ -2406,23 +2637,32 @@
       <c r="I27" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="3">
-        <v>1</v>
-      </c>
-      <c r="L27" s="3" t="s">
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>1980</v>
+      </c>
+      <c r="M27">
+        <v>2015</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="N27" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="O27" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P27" s="3">
+      <c r="R27" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S27" s="3">
         <v>2007</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>98</v>
       </c>
@@ -2444,8 +2684,13 @@
       <c r="I28" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K28" t="s">
+        <v>382</v>
+      </c>
+      <c r="L28"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>99</v>
       </c>
@@ -2476,20 +2721,29 @@
       <c r="J29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="K29" s="3">
-        <v>1</v>
-      </c>
-      <c r="L29" s="3" t="s">
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>1980</v>
+      </c>
+      <c r="M29">
+        <v>2009</v>
+      </c>
+      <c r="N29" s="3">
+        <v>1</v>
+      </c>
+      <c r="O29" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O29" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P29" s="3">
+      <c r="R29" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S29" s="3">
         <v>2009</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -2511,8 +2765,13 @@
       <c r="I30" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K30" t="s">
+        <v>382</v>
+      </c>
+      <c r="L30"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>105</v>
       </c>
@@ -2534,8 +2793,13 @@
       <c r="I31" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K31" t="s">
+        <v>382</v>
+      </c>
+      <c r="L31"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>106</v>
       </c>
@@ -2566,8 +2830,17 @@
       <c r="J32" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32">
+        <v>1980</v>
+      </c>
+      <c r="M32">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -2598,8 +2871,17 @@
       <c r="J33" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33">
+        <v>1980</v>
+      </c>
+      <c r="M33">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>111</v>
       </c>
@@ -2621,14 +2903,19 @@
       <c r="I34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K34" s="2">
-        <v>1</v>
-      </c>
-      <c r="M34" s="2" t="s">
+      <c r="K34" t="s">
+        <v>382</v>
+      </c>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34" s="2">
+        <v>1</v>
+      </c>
+      <c r="P34" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>112</v>
       </c>
@@ -2659,8 +2946,17 @@
       <c r="J35" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>1980</v>
+      </c>
+      <c r="M35">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>115</v>
       </c>
@@ -2685,8 +2981,17 @@
       <c r="I36" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>1980</v>
+      </c>
+      <c r="M36">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>118</v>
       </c>
@@ -2717,8 +3022,17 @@
       <c r="J37" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>1980</v>
+      </c>
+      <c r="M37">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>123</v>
       </c>
@@ -2749,8 +3063,17 @@
       <c r="J38" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K38">
+        <v>1</v>
+      </c>
+      <c r="L38">
+        <v>1980</v>
+      </c>
+      <c r="M38">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>127</v>
       </c>
@@ -2781,8 +3104,17 @@
       <c r="J39" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K39">
+        <v>1</v>
+      </c>
+      <c r="L39">
+        <v>1980</v>
+      </c>
+      <c r="M39">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>132</v>
       </c>
@@ -2807,8 +3139,17 @@
       <c r="I40" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K40">
+        <v>1</v>
+      </c>
+      <c r="L40">
+        <v>1980</v>
+      </c>
+      <c r="M40">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>135</v>
       </c>
@@ -2839,20 +3180,29 @@
       <c r="J41" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="K41" s="3">
-        <v>1</v>
-      </c>
-      <c r="L41" s="3" t="s">
+      <c r="K41">
+        <v>1</v>
+      </c>
+      <c r="L41">
+        <v>1980</v>
+      </c>
+      <c r="M41">
+        <v>2011</v>
+      </c>
+      <c r="N41" s="3">
+        <v>1</v>
+      </c>
+      <c r="O41" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O41" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P41" s="3">
+      <c r="R41" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S41" s="3">
         <v>2011</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>138</v>
       </c>
@@ -2883,8 +3233,17 @@
       <c r="J42" s="2" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K42">
+        <v>1</v>
+      </c>
+      <c r="L42">
+        <v>1980</v>
+      </c>
+      <c r="M42">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>143</v>
       </c>
@@ -2915,20 +3274,29 @@
       <c r="J43" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="K43" s="3">
-        <v>1</v>
-      </c>
-      <c r="L43" s="3" t="s">
+      <c r="K43">
+        <v>1</v>
+      </c>
+      <c r="L43">
+        <v>1980</v>
+      </c>
+      <c r="M43">
+        <v>2015</v>
+      </c>
+      <c r="N43" s="3">
+        <v>1</v>
+      </c>
+      <c r="O43" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O43" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P43" s="3">
+      <c r="R43" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S43" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>147</v>
       </c>
@@ -2959,20 +3327,29 @@
       <c r="J44" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="K44" s="3">
-        <v>1</v>
-      </c>
-      <c r="L44" s="3" t="s">
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44">
+        <v>1980</v>
+      </c>
+      <c r="M44">
+        <v>2008</v>
+      </c>
+      <c r="N44" s="3">
+        <v>1</v>
+      </c>
+      <c r="O44" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O44" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P44" s="3">
+      <c r="R44" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S44" s="3">
         <v>2008</v>
       </c>
     </row>
-    <row r="45" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>150</v>
       </c>
@@ -3003,20 +3380,29 @@
       <c r="J45" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="K45" s="3">
-        <v>1</v>
-      </c>
-      <c r="L45" s="3" t="s">
+      <c r="K45">
+        <v>1</v>
+      </c>
+      <c r="L45">
+        <v>1980</v>
+      </c>
+      <c r="M45">
+        <v>2013</v>
+      </c>
+      <c r="N45" s="3">
+        <v>1</v>
+      </c>
+      <c r="O45" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O45" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P45" s="3">
+      <c r="R45" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S45" s="3">
         <v>2013</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>155</v>
       </c>
@@ -3047,20 +3433,29 @@
       <c r="J46" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="K46" s="3">
-        <v>1</v>
-      </c>
-      <c r="L46" s="3" t="s">
+      <c r="K46">
+        <v>1</v>
+      </c>
+      <c r="L46">
+        <v>1981</v>
+      </c>
+      <c r="M46">
+        <v>2015</v>
+      </c>
+      <c r="N46" s="3">
+        <v>1</v>
+      </c>
+      <c r="O46" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O46" s="3">
+      <c r="R46" s="3">
         <v>1981</v>
       </c>
-      <c r="P46" s="3">
+      <c r="S46" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>158</v>
       </c>
@@ -3085,8 +3480,17 @@
       <c r="I47" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="48" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>1980</v>
+      </c>
+      <c r="M47">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>161</v>
       </c>
@@ -3111,20 +3515,29 @@
       <c r="I48" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K48" s="3">
-        <v>1</v>
-      </c>
-      <c r="L48" s="3" t="s">
+      <c r="K48">
+        <v>1</v>
+      </c>
+      <c r="L48">
+        <v>1980</v>
+      </c>
+      <c r="M48">
+        <v>2007</v>
+      </c>
+      <c r="N48" s="3">
+        <v>1</v>
+      </c>
+      <c r="O48" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O48" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P48" s="3">
+      <c r="R48" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S48" s="3">
         <v>2007</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>164</v>
       </c>
@@ -3146,8 +3559,13 @@
       <c r="I49" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K49" t="s">
+        <v>382</v>
+      </c>
+      <c r="L49"/>
+      <c r="M49"/>
+    </row>
+    <row r="50" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>165</v>
       </c>
@@ -3172,8 +3590,17 @@
       <c r="I50" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>1980</v>
+      </c>
+      <c r="M50">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>168</v>
       </c>
@@ -3204,8 +3631,17 @@
       <c r="J51" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="52" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>1980</v>
+      </c>
+      <c r="M51">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="52" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>171</v>
       </c>
@@ -3236,8 +3672,17 @@
       <c r="J52" s="2" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="53" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>1980</v>
+      </c>
+      <c r="M52">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>175</v>
       </c>
@@ -3268,20 +3713,29 @@
       <c r="J53" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="K53" s="3">
-        <v>1</v>
-      </c>
-      <c r="L53" s="3" t="s">
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>1980</v>
+      </c>
+      <c r="M53">
+        <v>2015</v>
+      </c>
+      <c r="N53" s="3">
+        <v>1</v>
+      </c>
+      <c r="O53" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O53" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P53" s="3">
+      <c r="R53" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S53" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>178</v>
       </c>
@@ -3303,8 +3757,13 @@
       <c r="I54" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K54" t="s">
+        <v>382</v>
+      </c>
+      <c r="L54"/>
+      <c r="M54"/>
+    </row>
+    <row r="55" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>179</v>
       </c>
@@ -3329,20 +3788,29 @@
       <c r="I55" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K55" s="3">
-        <v>1</v>
-      </c>
-      <c r="L55" s="3" t="s">
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>1980</v>
+      </c>
+      <c r="M55">
+        <v>2013</v>
+      </c>
+      <c r="N55" s="3">
+        <v>1</v>
+      </c>
+      <c r="O55" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O55" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P55" s="3">
+      <c r="R55" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S55" s="3">
         <v>2013</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>182</v>
       </c>
@@ -3373,8 +3841,17 @@
       <c r="J56" s="2" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>1980</v>
+      </c>
+      <c r="M56">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>185</v>
       </c>
@@ -3396,14 +3873,19 @@
       <c r="I57" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K57" s="2">
-        <v>1</v>
-      </c>
-      <c r="M57" s="2" t="s">
+      <c r="K57" t="s">
+        <v>382</v>
+      </c>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57" s="2">
+        <v>1</v>
+      </c>
+      <c r="P57" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>186</v>
       </c>
@@ -3425,14 +3907,19 @@
       <c r="I58" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K58" s="2">
-        <v>1</v>
-      </c>
-      <c r="M58" s="2" t="s">
+      <c r="K58" t="s">
+        <v>382</v>
+      </c>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58" s="2">
+        <v>1</v>
+      </c>
+      <c r="P58" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>187</v>
       </c>
@@ -3460,8 +3947,17 @@
       <c r="J59" s="2" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>1980</v>
+      </c>
+      <c r="M59">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>191</v>
       </c>
@@ -3492,14 +3988,23 @@
       <c r="J60" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="K60" s="2">
-        <v>1</v>
-      </c>
-      <c r="M60" s="2" t="s">
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>1980</v>
+      </c>
+      <c r="M60">
+        <v>2000</v>
+      </c>
+      <c r="N60" s="2">
+        <v>1</v>
+      </c>
+      <c r="P60" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>194</v>
       </c>
@@ -3527,8 +4032,17 @@
       <c r="J61" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="L61">
+        <v>1980</v>
+      </c>
+      <c r="M61">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>197</v>
       </c>
@@ -3559,20 +4073,29 @@
       <c r="J62" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="K62" s="3">
-        <v>1</v>
-      </c>
-      <c r="L62" s="3" t="s">
+      <c r="K62">
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <v>1980</v>
+      </c>
+      <c r="M62">
+        <v>2015</v>
+      </c>
+      <c r="N62" s="3">
+        <v>1</v>
+      </c>
+      <c r="O62" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="O62" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P62" s="3">
+      <c r="R62" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S62" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>203</v>
       </c>
@@ -3594,8 +4117,13 @@
       <c r="I63" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K63" t="s">
+        <v>382</v>
+      </c>
+      <c r="L63"/>
+      <c r="M63"/>
+    </row>
+    <row r="64" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>204</v>
       </c>
@@ -3617,14 +4145,19 @@
       <c r="I64" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K64" s="2">
-        <v>1</v>
-      </c>
-      <c r="M64" s="2" t="s">
+      <c r="K64" t="s">
+        <v>382</v>
+      </c>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64" s="2">
+        <v>1</v>
+      </c>
+      <c r="P64" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>205</v>
       </c>
@@ -3646,8 +4179,13 @@
       <c r="I65" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="66" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K65" t="s">
+        <v>382</v>
+      </c>
+      <c r="L65"/>
+      <c r="M65"/>
+    </row>
+    <row r="66" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>206</v>
       </c>
@@ -3678,8 +4216,17 @@
       <c r="J66" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="67" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="L66">
+        <v>1980</v>
+      </c>
+      <c r="M66">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="67" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>209</v>
       </c>
@@ -3710,20 +4257,29 @@
       <c r="J67" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="K67" s="3">
-        <v>1</v>
-      </c>
-      <c r="L67" s="3" t="s">
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="L67">
+        <v>1980</v>
+      </c>
+      <c r="M67">
+        <v>2012</v>
+      </c>
+      <c r="N67" s="3">
+        <v>1</v>
+      </c>
+      <c r="O67" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O67" s="3">
+      <c r="R67" s="3">
         <v>1982</v>
       </c>
-      <c r="P67" s="3">
+      <c r="S67" s="3">
         <v>2012</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>212</v>
       </c>
@@ -3745,8 +4301,13 @@
       <c r="I68" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="69" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K68" t="s">
+        <v>382</v>
+      </c>
+      <c r="L68"/>
+      <c r="M68"/>
+    </row>
+    <row r="69" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>213</v>
       </c>
@@ -3771,8 +4332,17 @@
       <c r="I69" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="70" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="L69">
+        <v>1980</v>
+      </c>
+      <c r="M69">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="70" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>216</v>
       </c>
@@ -3803,20 +4373,29 @@
       <c r="J70" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="K70" s="3">
-        <v>1</v>
-      </c>
-      <c r="L70" s="3" t="s">
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="L70">
+        <v>1980</v>
+      </c>
+      <c r="M70">
+        <v>2007</v>
+      </c>
+      <c r="N70" s="3">
+        <v>1</v>
+      </c>
+      <c r="O70" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O70" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P70" s="3">
+      <c r="R70" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S70" s="3">
         <v>2007</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>221</v>
       </c>
@@ -3847,8 +4426,17 @@
       <c r="J71" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="72" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <v>1980</v>
+      </c>
+      <c r="M71">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="72" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>226</v>
       </c>
@@ -3879,8 +4467,17 @@
       <c r="J72" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="73" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="L72">
+        <v>1980</v>
+      </c>
+      <c r="M72">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="73" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>230</v>
       </c>
@@ -3911,8 +4508,17 @@
       <c r="J73" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="74" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="L73">
+        <v>1980</v>
+      </c>
+      <c r="M73">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="74" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>233</v>
       </c>
@@ -3943,8 +4549,17 @@
       <c r="J74" s="2" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="75" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K74">
+        <v>1</v>
+      </c>
+      <c r="L74">
+        <v>1980</v>
+      </c>
+      <c r="M74">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="75" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>237</v>
       </c>
@@ -3975,8 +4590,17 @@
       <c r="J75" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="76" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K75">
+        <v>1</v>
+      </c>
+      <c r="L75">
+        <v>1980</v>
+      </c>
+      <c r="M75">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="76" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>242</v>
       </c>
@@ -4001,20 +4625,29 @@
       <c r="I76" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K76" s="3">
-        <v>1</v>
-      </c>
-      <c r="L76" s="3" t="s">
+      <c r="K76">
+        <v>1</v>
+      </c>
+      <c r="L76">
+        <v>1980</v>
+      </c>
+      <c r="M76">
+        <v>1997</v>
+      </c>
+      <c r="N76" s="3">
+        <v>1</v>
+      </c>
+      <c r="O76" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O76" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P76" s="3">
+      <c r="R76" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S76" s="3">
         <v>1997</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>245</v>
       </c>
@@ -4045,8 +4678,17 @@
       <c r="J77" s="2" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="78" spans="1:16" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="K77">
+        <v>1</v>
+      </c>
+      <c r="L77">
+        <v>1980</v>
+      </c>
+      <c r="M77">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>250</v>
       </c>
@@ -4077,20 +4719,29 @@
       <c r="J78" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="K78" s="3">
-        <v>1</v>
-      </c>
-      <c r="L78" s="3" t="s">
+      <c r="K78">
+        <v>2</v>
+      </c>
+      <c r="L78">
+        <v>1980</v>
+      </c>
+      <c r="M78">
+        <v>2015</v>
+      </c>
+      <c r="N78" s="3">
+        <v>1</v>
+      </c>
+      <c r="O78" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="O78" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P78" s="3">
+      <c r="R78" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S78" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>254</v>
       </c>
@@ -4112,8 +4763,13 @@
       <c r="I79" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="80" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K79" t="s">
+        <v>382</v>
+      </c>
+      <c r="L79"/>
+      <c r="M79"/>
+    </row>
+    <row r="80" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>255</v>
       </c>
@@ -4144,8 +4800,17 @@
       <c r="J80" s="2" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K80">
+        <v>1</v>
+      </c>
+      <c r="L80">
+        <v>1980</v>
+      </c>
+      <c r="M80">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="81" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>258</v>
       </c>
@@ -4176,20 +4841,29 @@
       <c r="J81" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="K81" s="3">
-        <v>1</v>
-      </c>
-      <c r="L81" s="3" t="s">
+      <c r="K81">
+        <v>1</v>
+      </c>
+      <c r="L81">
+        <v>1980</v>
+      </c>
+      <c r="M81">
+        <v>2015</v>
+      </c>
+      <c r="N81" s="3">
+        <v>1</v>
+      </c>
+      <c r="O81" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O81" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P81" s="3">
+      <c r="R81" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S81" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>262</v>
       </c>
@@ -4211,14 +4885,19 @@
       <c r="I82" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K82" s="2">
-        <v>1</v>
-      </c>
-      <c r="M82" s="2" t="s">
+      <c r="K82" t="s">
+        <v>382</v>
+      </c>
+      <c r="L82"/>
+      <c r="M82"/>
+      <c r="N82" s="2">
+        <v>1</v>
+      </c>
+      <c r="P82" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>263</v>
       </c>
@@ -4240,8 +4919,13 @@
       <c r="I83" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K83" t="s">
+        <v>382</v>
+      </c>
+      <c r="L83"/>
+      <c r="M83"/>
+    </row>
+    <row r="84" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>264</v>
       </c>
@@ -4269,8 +4953,17 @@
       <c r="I84" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K84">
+        <v>1</v>
+      </c>
+      <c r="L84">
+        <v>1980</v>
+      </c>
+      <c r="M84">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="85" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>267</v>
       </c>
@@ -4295,8 +4988,17 @@
       <c r="I85" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K85">
+        <v>1</v>
+      </c>
+      <c r="L85">
+        <v>1980</v>
+      </c>
+      <c r="M85">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="86" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>269</v>
       </c>
@@ -4327,8 +5029,17 @@
       <c r="J86" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K86">
+        <v>1</v>
+      </c>
+      <c r="L86">
+        <v>1980</v>
+      </c>
+      <c r="M86">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="87" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>272</v>
       </c>
@@ -4353,8 +5064,17 @@
       <c r="I87" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" ht="48" x14ac:dyDescent="0.2">
+      <c r="K87">
+        <v>1</v>
+      </c>
+      <c r="L87">
+        <v>1980</v>
+      </c>
+      <c r="M87">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="88" spans="1:19" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>275</v>
       </c>
@@ -4385,8 +5105,17 @@
       <c r="J88" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K88">
+        <v>1</v>
+      </c>
+      <c r="L88">
+        <v>1980</v>
+      </c>
+      <c r="M88">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="89" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>278</v>
       </c>
@@ -4417,8 +5146,17 @@
       <c r="J89" s="2" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89">
+        <v>1980</v>
+      </c>
+      <c r="M89">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="90" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>282</v>
       </c>
@@ -4443,8 +5181,17 @@
       <c r="I90" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K90">
+        <v>1</v>
+      </c>
+      <c r="L90">
+        <v>1980</v>
+      </c>
+      <c r="M90">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="91" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>285</v>
       </c>
@@ -4469,20 +5216,29 @@
       <c r="I91" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K91" s="3">
-        <v>1</v>
-      </c>
-      <c r="L91" s="3" t="s">
+      <c r="K91">
+        <v>1</v>
+      </c>
+      <c r="L91">
+        <v>1980</v>
+      </c>
+      <c r="M91">
+        <v>2002</v>
+      </c>
+      <c r="N91" s="3">
+        <v>1</v>
+      </c>
+      <c r="O91" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O91" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P91" s="3">
+      <c r="R91" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S91" s="3">
         <v>2002</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>287</v>
       </c>
@@ -4504,8 +5260,13 @@
       <c r="I92" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K92" t="s">
+        <v>382</v>
+      </c>
+      <c r="L92"/>
+      <c r="M92"/>
+    </row>
+    <row r="93" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>288</v>
       </c>
@@ -4530,8 +5291,17 @@
       <c r="I93" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="94" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K93">
+        <v>1</v>
+      </c>
+      <c r="L93">
+        <v>1980</v>
+      </c>
+      <c r="M93">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="94" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>290</v>
       </c>
@@ -4553,8 +5323,13 @@
       <c r="I94" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="95" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K94" t="s">
+        <v>382</v>
+      </c>
+      <c r="L94"/>
+      <c r="M94"/>
+    </row>
+    <row r="95" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>291</v>
       </c>
@@ -4579,8 +5354,17 @@
       <c r="I95" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K95">
+        <v>1</v>
+      </c>
+      <c r="L95">
+        <v>1980</v>
+      </c>
+      <c r="M95">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="96" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>293</v>
       </c>
@@ -4611,8 +5395,17 @@
       <c r="J96" s="2" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="97" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <v>1</v>
+      </c>
+      <c r="L96">
+        <v>1980</v>
+      </c>
+      <c r="M96">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="97" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>298</v>
       </c>
@@ -4637,8 +5430,17 @@
       <c r="I97" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="98" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <v>1</v>
+      </c>
+      <c r="L97">
+        <v>1980</v>
+      </c>
+      <c r="M97">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>300</v>
       </c>
@@ -4663,20 +5465,29 @@
       <c r="I98" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K98" s="3">
-        <v>1</v>
-      </c>
-      <c r="L98" s="3" t="s">
+      <c r="K98">
+        <v>1</v>
+      </c>
+      <c r="L98">
+        <v>1986</v>
+      </c>
+      <c r="M98">
+        <v>2015</v>
+      </c>
+      <c r="N98" s="3">
+        <v>1</v>
+      </c>
+      <c r="O98" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O98" s="3">
+      <c r="R98" s="3">
         <v>1986</v>
       </c>
-      <c r="P98" s="3">
+      <c r="S98" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>302</v>
       </c>
@@ -4707,8 +5518,17 @@
       <c r="J99" s="2" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="100" spans="1:16" ht="32" x14ac:dyDescent="0.2">
+      <c r="K99">
+        <v>1</v>
+      </c>
+      <c r="L99">
+        <v>1980</v>
+      </c>
+      <c r="M99">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="100" spans="1:19" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>304</v>
       </c>
@@ -4739,8 +5559,17 @@
       <c r="J100" s="2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="101" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K100">
+        <v>1</v>
+      </c>
+      <c r="L100">
+        <v>1980</v>
+      </c>
+      <c r="M100">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="101" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>309</v>
       </c>
@@ -4765,20 +5594,29 @@
       <c r="I101" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K101" s="3">
-        <v>1</v>
-      </c>
-      <c r="L101" s="3" t="s">
+      <c r="K101">
+        <v>1</v>
+      </c>
+      <c r="L101">
+        <v>1985</v>
+      </c>
+      <c r="M101">
+        <v>2015</v>
+      </c>
+      <c r="N101" s="3">
+        <v>1</v>
+      </c>
+      <c r="O101" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O101" s="3">
+      <c r="R101" s="3">
         <v>1985</v>
       </c>
-      <c r="P101" s="3">
+      <c r="S101" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>312</v>
       </c>
@@ -4809,8 +5647,17 @@
       <c r="J102" s="2" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="103" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K102">
+        <v>1</v>
+      </c>
+      <c r="L102">
+        <v>1980</v>
+      </c>
+      <c r="M102">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="103" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>316</v>
       </c>
@@ -4835,8 +5682,17 @@
       <c r="I103" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="104" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <v>1</v>
+      </c>
+      <c r="L103">
+        <v>1980</v>
+      </c>
+      <c r="M103">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="104" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>318</v>
       </c>
@@ -4867,8 +5723,17 @@
       <c r="J104" s="2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="105" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="K104">
+        <v>1</v>
+      </c>
+      <c r="L104">
+        <v>1980</v>
+      </c>
+      <c r="M104">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="105" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>321</v>
       </c>
@@ -4893,58 +5758,76 @@
       <c r="I105" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K105" s="3">
-        <v>1</v>
-      </c>
-      <c r="L105" s="3" t="s">
+      <c r="K105">
+        <v>1</v>
+      </c>
+      <c r="L105">
+        <v>1985</v>
+      </c>
+      <c r="M105">
+        <v>2015</v>
+      </c>
+      <c r="N105" s="3">
+        <v>1</v>
+      </c>
+      <c r="O105" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O105" s="3">
+      <c r="R105" s="3">
         <v>1985</v>
       </c>
-      <c r="P105" s="3">
+      <c r="S105" s="3">
         <v>2015</v>
       </c>
     </row>
-    <row r="106" spans="1:16" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A106" s="4" t="s">
+    <row r="106" spans="1:19" ht="16" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="B106" s="4">
+      <c r="B106" s="2">
         <v>20145</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D106" s="4" t="s">
+      <c r="D106" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="E106" s="4">
-        <v>0</v>
-      </c>
-      <c r="F106" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H106" s="4">
-        <v>0</v>
-      </c>
-      <c r="I106" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K106" s="4">
-        <v>1</v>
-      </c>
-      <c r="M106" s="4" t="s">
+      <c r="E106" s="2">
+        <v>0</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H106" s="2">
+        <v>0</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K106">
+        <v>1</v>
+      </c>
+      <c r="L106">
+        <v>1980</v>
+      </c>
+      <c r="M106">
+        <v>2002</v>
+      </c>
+      <c r="N106" s="2">
+        <v>1</v>
+      </c>
+      <c r="P106" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="O106" s="4">
-        <v>1980</v>
-      </c>
-      <c r="P106" s="4">
+      <c r="R106" s="2">
+        <v>1980</v>
+      </c>
+      <c r="S106" s="2">
         <v>2002</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>326</v>
       </c>
@@ -4966,8 +5849,13 @@
       <c r="I107" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="108" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K107" t="s">
+        <v>382</v>
+      </c>
+      <c r="L107"/>
+      <c r="M107"/>
+    </row>
+    <row r="108" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>327</v>
       </c>
@@ -4992,8 +5880,17 @@
       <c r="I108" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="109" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <v>1</v>
+      </c>
+      <c r="L108">
+        <v>1980</v>
+      </c>
+      <c r="M108">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="109" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>329</v>
       </c>
@@ -5018,8 +5915,17 @@
       <c r="I109" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="110" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <v>1</v>
+      </c>
+      <c r="L109">
+        <v>1980</v>
+      </c>
+      <c r="M109">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="110" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>332</v>
       </c>
@@ -5050,8 +5956,17 @@
       <c r="J110" s="2" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="111" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <v>1</v>
+      </c>
+      <c r="L110">
+        <v>1980</v>
+      </c>
+      <c r="M110">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="111" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>336</v>
       </c>
@@ -5082,8 +5997,17 @@
       <c r="J111" s="2" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="112" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <v>1</v>
+      </c>
+      <c r="L111">
+        <v>1980</v>
+      </c>
+      <c r="M111">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="112" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>338</v>
       </c>
@@ -5108,8 +6032,17 @@
       <c r="I112" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="113" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K112">
+        <v>1</v>
+      </c>
+      <c r="L112">
+        <v>1980</v>
+      </c>
+      <c r="M112">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>340</v>
       </c>
@@ -5131,8 +6064,13 @@
       <c r="I113" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="114" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K113" t="s">
+        <v>382</v>
+      </c>
+      <c r="L113"/>
+      <c r="M113"/>
+    </row>
+    <row r="114" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>341</v>
       </c>
@@ -5157,8 +6095,17 @@
       <c r="I114" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="115" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K114">
+        <v>1</v>
+      </c>
+      <c r="L114">
+        <v>1987</v>
+      </c>
+      <c r="M114">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="115" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>344</v>
       </c>
@@ -5180,14 +6127,19 @@
       <c r="I115" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K115" s="2">
-        <v>1</v>
-      </c>
-      <c r="M115" s="2" t="s">
+      <c r="K115" t="s">
+        <v>382</v>
+      </c>
+      <c r="L115"/>
+      <c r="M115"/>
+      <c r="N115" s="2">
+        <v>1</v>
+      </c>
+      <c r="P115" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="116" spans="1:16" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:19" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>345</v>
       </c>
@@ -5212,23 +6164,32 @@
       <c r="I116" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K116" s="3">
-        <v>1</v>
-      </c>
-      <c r="L116" s="3" t="s">
+      <c r="K116">
+        <v>1</v>
+      </c>
+      <c r="L116">
+        <v>1980</v>
+      </c>
+      <c r="M116">
+        <v>2004</v>
+      </c>
+      <c r="N116" s="3">
+        <v>1</v>
+      </c>
+      <c r="O116" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="N116" s="3" t="s">
+      <c r="Q116" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="O116" s="3">
+      <c r="R116" s="3">
         <v>1991</v>
       </c>
-      <c r="P116" s="3">
+      <c r="S116" s="3">
         <v>2003</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>348</v>
       </c>
@@ -5250,14 +6211,19 @@
       <c r="I117" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K117" s="2">
-        <v>1</v>
-      </c>
-      <c r="M117" s="2" t="s">
+      <c r="K117" t="s">
+        <v>382</v>
+      </c>
+      <c r="L117"/>
+      <c r="M117"/>
+      <c r="N117" s="2">
+        <v>1</v>
+      </c>
+      <c r="P117" s="2" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>349</v>
       </c>
@@ -5282,8 +6248,17 @@
       <c r="I118" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="119" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K118">
+        <v>1</v>
+      </c>
+      <c r="L118">
+        <v>1980</v>
+      </c>
+      <c r="M118">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="119" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>352</v>
       </c>
@@ -5308,14 +6283,23 @@
       <c r="I119" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K119" s="2">
-        <v>1</v>
-      </c>
-      <c r="M119" s="2" t="s">
+      <c r="K119">
+        <v>1</v>
+      </c>
+      <c r="L119">
+        <v>1980</v>
+      </c>
+      <c r="M119">
+        <v>2009</v>
+      </c>
+      <c r="N119" s="2">
+        <v>1</v>
+      </c>
+      <c r="P119" s="2" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>355</v>
       </c>
@@ -5346,8 +6330,17 @@
       <c r="J120" s="2" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="121" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="K120">
+        <v>1</v>
+      </c>
+      <c r="L120">
+        <v>1980</v>
+      </c>
+      <c r="M120">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="121" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>359</v>
       </c>
@@ -5378,8 +6371,17 @@
       <c r="J121" s="2" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="122" spans="1:16" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>1980</v>
+      </c>
+      <c r="M121">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="122" spans="1:19" s="3" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
         <v>362</v>
       </c>
@@ -5410,16 +6412,25 @@
       <c r="J122" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="K122" s="3">
-        <v>1</v>
-      </c>
-      <c r="L122" s="3" t="s">
+      <c r="K122">
+        <v>1</v>
+      </c>
+      <c r="L122">
+        <v>1980</v>
+      </c>
+      <c r="M122">
+        <v>2015</v>
+      </c>
+      <c r="N122" s="3">
+        <v>1</v>
+      </c>
+      <c r="O122" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="O122" s="3">
-        <v>1980</v>
-      </c>
-      <c r="P122" s="3">
+      <c r="R122" s="3">
+        <v>1980</v>
+      </c>
+      <c r="S122" s="3">
         <v>2015</v>
       </c>
     </row>

</xml_diff>